<commit_message>
Removed files and added to new website
</commit_message>
<xml_diff>
--- a/Administration/Website Revision Timeline.xlsx
+++ b/Administration/Website Revision Timeline.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2C3FFB-9DDC-4A4D-9D7C-EDB558CF1B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3648175-E6E0-4AEC-B0DE-309045FA8176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="2460" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7170" yWindow="2910" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -911,6 +911,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -922,12 +928,6 @@
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1546,106 +1546,106 @@
       <c r="B3" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="91">
+      <c r="D3" s="89"/>
+      <c r="E3" s="93">
         <v>44793</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="93"/>
+      <c r="D4" s="89"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="90">
         <f>I5</f>
         <v>44788</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
         <f>P5</f>
         <v>44795</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
         <f>W5</f>
         <v>44802</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
         <f>AD5</f>
         <v>44809</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
         <f>AK5</f>
         <v>44816</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
         <f>AR5</f>
         <v>44823</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
         <f>AY5</f>
         <v>44830</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
         <f>BF5</f>
         <v>44837</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
@@ -3880,17 +3880,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D30">
     <cfRule type="dataBar" priority="14">
@@ -4058,6 +4058,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE32FFEA2BDF7847939D87CA8C34DA4E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0306461de4e0b58e31eb036a11d72f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8007b371-3734-4ab8-9a57-97cc26f1b7d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9115aebfdb12be3b5c968ebb0f603b76" ns3:_="">
     <xsd:import namespace="8007b371-3734-4ab8-9a57-97cc26f1b7d2"/>
@@ -4203,35 +4218,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03BA4B9A-3432-4495-891B-6D6ECA9E9929}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86903AC-B483-4B6E-9F6B-19FCB8CD5534}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8007b371-3734-4ab8-9a57-97cc26f1b7d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4253,9 +4243,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E86903AC-B483-4B6E-9F6B-19FCB8CD5534}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03BA4B9A-3432-4495-891B-6D6ECA9E9929}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8007b371-3734-4ab8-9a57-97cc26f1b7d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>